<commit_message>
Fixing evaluation dataset issue
</commit_message>
<xml_diff>
--- a/Datasets/01 Datasets - used in training/Dataset Stats.xlsx
+++ b/Datasets/01 Datasets - used in training/Dataset Stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Christian/Documents/1 Studium/1 Master Unterlagen/01 WS1920/Projekt ISE/DBpedia_Img2Ent/Datasets/01 Datasets - used in training/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/17/k6x70_j11h55lxsd41xx0fpr0000gn/T/BDDB7B53-7D21-4BE7-9A09-1CF14EC565F6/Datasets/01 Datasets - used in training/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AF9A0E-83FA-3840-BADB-DE91D39C692D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744A8869-3046-EC4D-9079-2E485DA6D76E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="23540" xr2:uid="{D584A97D-CA79-CC48-9BA2-6927C9B78ED7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="318">
   <si>
     <t>AdministrativeRegion</t>
   </si>
@@ -335,9 +335,6 @@
     <t>WrittenWork</t>
   </si>
   <si>
-    <t>AcademicConference</t>
-  </si>
-  <si>
     <t>AcademicJournal</t>
   </si>
   <si>
@@ -371,9 +368,6 @@
     <t>Artwork</t>
   </si>
   <si>
-    <t>AustralianFootballTeam</t>
-  </si>
-  <si>
     <t>Bacteria</t>
   </si>
   <si>
@@ -386,9 +380,6 @@
     <t>BaseballTeam</t>
   </si>
   <si>
-    <t>BasketballLeague</t>
-  </si>
-  <si>
     <t>BasketballTeam</t>
   </si>
   <si>
@@ -440,9 +431,6 @@
     <t>Comedian</t>
   </si>
   <si>
-    <t>ComedyGroup</t>
-  </si>
-  <si>
     <t>Comic</t>
   </si>
   <si>
@@ -638,9 +626,6 @@
     <t>NascarDriver</t>
   </si>
   <si>
-    <t>NationalFootballLeagueEvent</t>
-  </si>
-  <si>
     <t>Newspaper</t>
   </si>
   <si>
@@ -677,9 +662,6 @@
     <t>Poet</t>
   </si>
   <si>
-    <t>PoloLeague</t>
-  </si>
-  <si>
     <t>PowerStation</t>
   </si>
   <si>
@@ -737,9 +719,6 @@
     <t>SiteOfSpecialScientificInterest</t>
   </si>
   <si>
-    <t>Skater</t>
-  </si>
-  <si>
     <t>SkiArea</t>
   </si>
   <si>
@@ -755,9 +734,6 @@
     <t>SoapCharacter</t>
   </si>
   <si>
-    <t>SoccerLeague</t>
-  </si>
-  <si>
     <t>SoccerManager</t>
   </si>
   <si>
@@ -767,9 +743,6 @@
     <t>Song</t>
   </si>
   <si>
-    <t>SpaceStation</t>
-  </si>
-  <si>
     <t>SportsEvent</t>
   </si>
   <si>
@@ -824,18 +797,12 @@
     <t>Website</t>
   </si>
   <si>
-    <t>WomensTennisAssociationTournament</t>
-  </si>
-  <si>
     <t>Wrestler</t>
   </si>
   <si>
     <t>WrestlingEvent</t>
   </si>
   <si>
-    <t>The images were scraped regarding the 100 rdf types used in the training datasets. Then, the most specific rdf:type was assigned to each image. The classification models are not trained on all of them, but in the calculation of the evaluation metrics all parent classes are regarded as well. This ensures that the classifiers have the chance to classify as specific as possible.</t>
-  </si>
-  <si>
     <t>01 Large</t>
   </si>
   <si>
@@ -846,6 +813,180 @@
   </si>
   <si>
     <t>05 Evaluation (most specific class)</t>
+  </si>
+  <si>
+    <t>The images are a combination of the test-images of the other datasets, excluding images that appear in training dataset. The most specific rdf:type is assigned to each image. The classification models are trained on only the top 100 classes, but in the calculation of the evaluation metrics all classes and their hierarchies are regarded. This ensures that the classifiers have the chance to classify as specific as possible.</t>
+  </si>
+  <si>
+    <t>Airline</t>
+  </si>
+  <si>
+    <t>AmericanFootballPlayer</t>
+  </si>
+  <si>
+    <t>Amphibian</t>
+  </si>
+  <si>
+    <t>Arachnid</t>
+  </si>
+  <si>
+    <t>ArtificialSatellite</t>
+  </si>
+  <si>
+    <t>AutomobileEngine</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>Beverage</t>
+  </si>
+  <si>
+    <t>Brewery</t>
+  </si>
+  <si>
+    <t>BroadcastNetwork</t>
+  </si>
+  <si>
+    <t>BusCompany</t>
+  </si>
+  <si>
+    <t>Canal</t>
+  </si>
+  <si>
+    <t>Cardinal</t>
+  </si>
+  <si>
+    <t>Castle</t>
+  </si>
+  <si>
+    <t>Cheese</t>
+  </si>
+  <si>
+    <t>ChristianBishop</t>
+  </si>
+  <si>
+    <t>Conifer</t>
+  </si>
+  <si>
+    <t>Constellation</t>
+  </si>
+  <si>
+    <t>Crustacean</t>
+  </si>
+  <si>
+    <t>CultivatedVariety</t>
+  </si>
+  <si>
+    <t>Cycad</t>
+  </si>
+  <si>
+    <t>Diocese</t>
+  </si>
+  <si>
+    <t>Drug</t>
+  </si>
+  <si>
+    <t>Fern</t>
+  </si>
+  <si>
+    <t>FloweringPlant</t>
+  </si>
+  <si>
+    <t>Fungus</t>
+  </si>
+  <si>
+    <t>Galaxy</t>
+  </si>
+  <si>
+    <t>Gnetophytes</t>
+  </si>
+  <si>
+    <t>Grape</t>
+  </si>
+  <si>
+    <t>GreenAlga</t>
+  </si>
+  <si>
+    <t>Horse</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>Hotel</t>
+  </si>
+  <si>
+    <t>InformationAppliance</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>Mineral</t>
+  </si>
+  <si>
+    <t>Moss</t>
+  </si>
+  <si>
+    <t>Museum</t>
+  </si>
+  <si>
+    <t>Planet</t>
+  </si>
+  <si>
+    <t>Pope</t>
+  </si>
+  <si>
+    <t>Prison</t>
+  </si>
+  <si>
+    <t>PublicTransitSystem</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>RadioStation</t>
+  </si>
+  <si>
+    <t>RecordLabel</t>
+  </si>
+  <si>
+    <t>ReligiousBuilding</t>
+  </si>
+  <si>
+    <t>Reptile</t>
+  </si>
+  <si>
+    <t>Restaurant</t>
+  </si>
+  <si>
+    <t>Saint</t>
+  </si>
+  <si>
+    <t>Sea</t>
+  </si>
+  <si>
+    <t>ShoppingMall</t>
+  </si>
+  <si>
+    <t>Star</t>
+  </si>
+  <si>
+    <t>TelevisionStation</t>
+  </si>
+  <si>
+    <t>Theatre</t>
+  </si>
+  <si>
+    <t>Venue</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Winery</t>
   </si>
 </sst>
 </file>
@@ -1221,10 +1362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0224D83A-02B0-AE4C-995A-515F93032E89}">
-  <dimension ref="A1:XFD224"/>
+  <dimension ref="A1:XFD310"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1245,19 +1386,19 @@
     </row>
     <row r="2" spans="1:12 16384:16384" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1277,11 +1418,11 @@
       <c r="D3">
         <v>9998</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>100</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:12 16384:16384" x14ac:dyDescent="0.2">
@@ -1297,11 +1438,11 @@
       <c r="D4">
         <v>8022</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>101</v>
       </c>
       <c r="G4">
-        <v>320</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:12 16384:16384" x14ac:dyDescent="0.2">
@@ -1317,11 +1458,11 @@
       <c r="D5">
         <v>6254</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>102</v>
+      <c r="F5" t="s">
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>28</v>
+        <v>425</v>
       </c>
     </row>
     <row r="6" spans="1:12 16384:16384" x14ac:dyDescent="0.2">
@@ -1337,11 +1478,11 @@
       <c r="D6">
         <v>10000</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>103</v>
+      <c r="F6" t="s">
+        <v>102</v>
       </c>
       <c r="G6">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:12 16384:16384" x14ac:dyDescent="0.2">
@@ -1357,11 +1498,11 @@
       <c r="D7">
         <v>10000</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>104</v>
+      <c r="F7" t="s">
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:12 16384:16384" x14ac:dyDescent="0.2">
@@ -1377,11 +1518,11 @@
       <c r="D8">
         <v>10000</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>105</v>
+      <c r="F8" t="s">
+        <v>261</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:12 16384:16384" x14ac:dyDescent="0.2">
@@ -1397,11 +1538,11 @@
       <c r="D9">
         <v>10000</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>106</v>
+      <c r="F9" t="s">
+        <v>2</v>
       </c>
       <c r="G9">
-        <v>14</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:12 16384:16384" x14ac:dyDescent="0.2">
@@ -1417,11 +1558,11 @@
       <c r="D10">
         <v>10000</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>107</v>
+      <c r="F10" t="s">
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>5</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="11" spans="1:12 16384:16384" x14ac:dyDescent="0.2">
@@ -1437,8 +1578,8 @@
       <c r="D11">
         <v>2185</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>108</v>
+      <c r="F11" t="s">
+        <v>103</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1457,11 +1598,11 @@
       <c r="D12">
         <v>7976</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>109</v>
+      <c r="F12" t="s">
+        <v>262</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:12 16384:16384" x14ac:dyDescent="0.2">
@@ -1477,11 +1618,11 @@
       <c r="D13">
         <v>4107</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>5</v>
+      <c r="F13" t="s">
+        <v>263</v>
       </c>
       <c r="G13">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1500,11 +1641,11 @@
       <c r="D14">
         <v>10000</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>6</v>
+      <c r="F14" t="s">
+        <v>104</v>
       </c>
       <c r="G14">
-        <v>209</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:12 16384:16384" x14ac:dyDescent="0.2">
@@ -1520,11 +1661,11 @@
       <c r="D15">
         <v>9998</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>110</v>
+      <c r="F15" t="s">
+        <v>4</v>
       </c>
       <c r="G15">
-        <v>32</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:12 16384:16384" x14ac:dyDescent="0.2">
@@ -1540,11 +1681,11 @@
       <c r="D16">
         <v>4275</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>111</v>
+      <c r="F16" t="s">
+        <v>105</v>
       </c>
       <c r="G16">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1560,11 +1701,11 @@
       <c r="D17">
         <v>10000</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>7</v>
+      <c r="F17" t="s">
+        <v>106</v>
       </c>
       <c r="G17">
-        <v>69</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1580,11 +1721,11 @@
       <c r="D18">
         <v>10000</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>112</v>
+      <c r="F18" t="s">
+        <v>264</v>
       </c>
       <c r="G18">
-        <v>9</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1600,11 +1741,11 @@
       <c r="D19">
         <v>10000</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>8</v>
+      <c r="F19" t="s">
+        <v>107</v>
       </c>
       <c r="G19">
-        <v>258</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1620,11 +1761,11 @@
       <c r="D20">
         <v>8587</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>9</v>
+      <c r="F20" t="s">
+        <v>108</v>
       </c>
       <c r="G20">
-        <v>1159</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1640,11 +1781,11 @@
       <c r="D21">
         <v>9999</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>10</v>
+      <c r="F21" t="s">
+        <v>5</v>
       </c>
       <c r="G21">
-        <v>473</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1660,11 +1801,11 @@
       <c r="D22">
         <v>5177</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>113</v>
+      <c r="F22" t="s">
+        <v>265</v>
       </c>
       <c r="G22">
-        <v>2</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1680,11 +1821,11 @@
       <c r="D23">
         <v>2969</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>114</v>
+      <c r="F23" t="s">
+        <v>6</v>
       </c>
       <c r="G23">
-        <v>3</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1700,11 +1841,11 @@
       <c r="D24">
         <v>3542</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>115</v>
+      <c r="F24" t="s">
+        <v>109</v>
       </c>
       <c r="G24">
-        <v>99</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1720,11 +1861,11 @@
       <c r="D25">
         <v>10000</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>116</v>
+      <c r="F25" t="s">
+        <v>110</v>
       </c>
       <c r="G25">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1740,11 +1881,11 @@
       <c r="D26">
         <v>9570</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>117</v>
+      <c r="F26" t="s">
+        <v>7</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1760,11 +1901,11 @@
       <c r="D27">
         <v>10000</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>118</v>
+      <c r="F27" t="s">
+        <v>8</v>
       </c>
       <c r="G27">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1780,11 +1921,11 @@
       <c r="D28">
         <v>3652</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>119</v>
+      <c r="F28" t="s">
+        <v>9</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1800,11 +1941,11 @@
       <c r="D29">
         <v>4106</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>120</v>
+      <c r="F29" t="s">
+        <v>266</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1820,11 +1961,11 @@
       <c r="D30">
         <v>8600</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>121</v>
+      <c r="F30" t="s">
+        <v>10</v>
       </c>
       <c r="G30">
-        <v>3</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1840,11 +1981,11 @@
       <c r="D31">
         <v>5975</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>122</v>
+      <c r="F31" t="s">
+        <v>111</v>
       </c>
       <c r="G31">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1860,11 +2001,11 @@
       <c r="D32">
         <v>9966</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>123</v>
+      <c r="F32" t="s">
+        <v>112</v>
       </c>
       <c r="G32">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1880,11 +2021,11 @@
       <c r="D33">
         <v>9999</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>124</v>
+      <c r="F33" t="s">
+        <v>11</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>420</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1900,11 +2041,11 @@
       <c r="D34">
         <v>10000</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>125</v>
+      <c r="F34" t="s">
+        <v>267</v>
       </c>
       <c r="G34">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1920,11 +2061,11 @@
       <c r="D35">
         <v>10000</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>126</v>
+      <c r="F35" t="s">
+        <v>113</v>
       </c>
       <c r="G35">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1940,11 +2081,11 @@
       <c r="D36">
         <v>10000</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>127</v>
+      <c r="F36" t="s">
+        <v>12</v>
       </c>
       <c r="G36">
-        <v>13</v>
+        <v>485</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1960,11 +2101,11 @@
       <c r="D37">
         <v>10000</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>128</v>
+      <c r="F37" t="s">
+        <v>114</v>
       </c>
       <c r="G37">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1980,11 +2121,11 @@
       <c r="D38">
         <v>9999</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>129</v>
+      <c r="F38" t="s">
+        <v>13</v>
       </c>
       <c r="G38">
-        <v>4</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -2000,11 +2141,11 @@
       <c r="D39">
         <v>8040</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>130</v>
+      <c r="F39" t="s">
+        <v>115</v>
       </c>
       <c r="G39">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -2020,11 +2161,11 @@
       <c r="D40">
         <v>7065</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>131</v>
+      <c r="F40" t="s">
+        <v>116</v>
       </c>
       <c r="G40">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -2040,11 +2181,11 @@
       <c r="D41">
         <v>9999</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>132</v>
+      <c r="F41" t="s">
+        <v>117</v>
       </c>
       <c r="G41">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -2060,11 +2201,11 @@
       <c r="D42">
         <v>9997</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>133</v>
+      <c r="F42" t="s">
+        <v>268</v>
       </c>
       <c r="G42">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -2080,11 +2221,11 @@
       <c r="D43">
         <v>10000</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>134</v>
+      <c r="F43" t="s">
+        <v>14</v>
       </c>
       <c r="G43">
-        <v>17</v>
+        <v>360</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -2100,11 +2241,11 @@
       <c r="D44">
         <v>6602</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>135</v>
+      <c r="F44" t="s">
+        <v>118</v>
       </c>
       <c r="G44">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -2120,11 +2261,11 @@
       <c r="D45">
         <v>9998</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>136</v>
+      <c r="F45" t="s">
+        <v>15</v>
       </c>
       <c r="G45">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -2140,11 +2281,11 @@
       <c r="D46">
         <v>10000</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>137</v>
+      <c r="F46" t="s">
+        <v>16</v>
       </c>
       <c r="G46">
-        <v>4</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -2160,11 +2301,11 @@
       <c r="D47">
         <v>5814</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>138</v>
+      <c r="F47" t="s">
+        <v>119</v>
       </c>
       <c r="G47">
-        <v>221</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -2180,11 +2321,11 @@
       <c r="D48">
         <v>6752</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>139</v>
+      <c r="F48" t="s">
+        <v>269</v>
       </c>
       <c r="G48">
-        <v>31</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -2200,11 +2341,11 @@
       <c r="D49">
         <v>2412</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>140</v>
+      <c r="F49" t="s">
+        <v>120</v>
       </c>
       <c r="G49">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -2220,11 +2361,11 @@
       <c r="D50">
         <v>9053</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>141</v>
+      <c r="F50" t="s">
+        <v>17</v>
       </c>
       <c r="G50">
-        <v>59</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -2240,11 +2381,11 @@
       <c r="D51">
         <v>9179</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>142</v>
+      <c r="F51" t="s">
+        <v>270</v>
       </c>
       <c r="G51">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -2260,11 +2401,11 @@
       <c r="D52">
         <v>10000</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>143</v>
+      <c r="F52" t="s">
+        <v>18</v>
       </c>
       <c r="G52">
-        <v>10</v>
+        <v>949</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -2280,11 +2421,11 @@
       <c r="D53">
         <v>10000</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>144</v>
+      <c r="F53" t="s">
+        <v>271</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -2300,11 +2441,11 @@
       <c r="D54">
         <v>9986</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>145</v>
+      <c r="F54" t="s">
+        <v>121</v>
       </c>
       <c r="G54">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -2320,8 +2461,8 @@
       <c r="D55">
         <v>10000</v>
       </c>
-      <c r="F55" s="1" t="s">
-        <v>146</v>
+      <c r="F55" t="s">
+        <v>122</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -2340,11 +2481,11 @@
       <c r="D56">
         <v>9998</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>147</v>
+      <c r="F56" t="s">
+        <v>272</v>
       </c>
       <c r="G56">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -2360,11 +2501,11 @@
       <c r="D57">
         <v>9999</v>
       </c>
-      <c r="F57" s="1" t="s">
-        <v>148</v>
+      <c r="F57" t="s">
+        <v>123</v>
       </c>
       <c r="G57">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -2380,11 +2521,11 @@
       <c r="D58">
         <v>10000</v>
       </c>
-      <c r="F58" s="1" t="s">
-        <v>149</v>
+      <c r="F58" t="s">
+        <v>273</v>
       </c>
       <c r="G58">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -2400,11 +2541,11 @@
       <c r="D59">
         <v>10000</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>150</v>
+      <c r="F59" t="s">
+        <v>274</v>
       </c>
       <c r="G59">
-        <v>69</v>
+        <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -2420,11 +2561,11 @@
       <c r="D60">
         <v>9735</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>151</v>
+      <c r="F60" t="s">
+        <v>124</v>
       </c>
       <c r="G60">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -2440,8 +2581,8 @@
       <c r="D61">
         <v>9993</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>152</v>
+      <c r="F61" t="s">
+        <v>125</v>
       </c>
       <c r="G61">
         <v>2</v>
@@ -2460,11 +2601,11 @@
       <c r="D62">
         <v>8195</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>153</v>
+      <c r="F62" t="s">
+        <v>275</v>
       </c>
       <c r="G62">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -2480,11 +2621,11 @@
       <c r="D63">
         <v>10000</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>154</v>
+      <c r="F63" t="s">
+        <v>20</v>
       </c>
       <c r="G63">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -2500,11 +2641,11 @@
       <c r="D64">
         <v>10000</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>32</v>
+      <c r="F64" t="s">
+        <v>21</v>
       </c>
       <c r="G64">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -2520,11 +2661,11 @@
       <c r="D65">
         <v>10000</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>155</v>
+      <c r="F65" t="s">
+        <v>126</v>
       </c>
       <c r="G65">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -2540,11 +2681,11 @@
       <c r="D66">
         <v>3125</v>
       </c>
-      <c r="F66" s="1" t="s">
-        <v>33</v>
+      <c r="F66" t="s">
+        <v>276</v>
       </c>
       <c r="G66">
-        <v>602</v>
+        <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -2560,11 +2701,11 @@
       <c r="D67">
         <v>10000</v>
       </c>
-      <c r="F67" s="1" t="s">
-        <v>156</v>
+      <c r="F67" t="s">
+        <v>22</v>
       </c>
       <c r="G67">
-        <v>132</v>
+        <v>491</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -2580,11 +2721,11 @@
       <c r="D68">
         <v>10000</v>
       </c>
-      <c r="F68" s="1" t="s">
-        <v>34</v>
+      <c r="F68" t="s">
+        <v>127</v>
       </c>
       <c r="G68">
-        <v>1223</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -2600,11 +2741,11 @@
       <c r="D69">
         <v>8278</v>
       </c>
-      <c r="F69" s="1" t="s">
-        <v>157</v>
+      <c r="F69" t="s">
+        <v>128</v>
       </c>
       <c r="G69">
-        <v>33</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -2620,11 +2761,11 @@
       <c r="D70">
         <v>5526</v>
       </c>
-      <c r="F70" s="1" t="s">
-        <v>158</v>
+      <c r="F70" t="s">
+        <v>23</v>
       </c>
       <c r="G70">
-        <v>55</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -2640,8 +2781,8 @@
       <c r="D71">
         <v>9999</v>
       </c>
-      <c r="F71" s="1" t="s">
-        <v>159</v>
+      <c r="F71" t="s">
+        <v>129</v>
       </c>
       <c r="G71">
         <v>2</v>
@@ -2660,11 +2801,11 @@
       <c r="D72">
         <v>9997</v>
       </c>
-      <c r="F72" s="1" t="s">
-        <v>160</v>
+      <c r="F72" t="s">
+        <v>130</v>
       </c>
       <c r="G72">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -2680,11 +2821,11 @@
       <c r="D73">
         <v>10000</v>
       </c>
-      <c r="F73" s="1" t="s">
-        <v>161</v>
+      <c r="F73" t="s">
+        <v>131</v>
       </c>
       <c r="G73">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -2700,11 +2841,11 @@
       <c r="D74">
         <v>10000</v>
       </c>
-      <c r="F74" s="1" t="s">
-        <v>162</v>
+      <c r="F74" t="s">
+        <v>132</v>
       </c>
       <c r="G74">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -2720,11 +2861,11 @@
       <c r="D75">
         <v>7516</v>
       </c>
-      <c r="F75" s="1" t="s">
-        <v>163</v>
+      <c r="F75" t="s">
+        <v>134</v>
       </c>
       <c r="G75">
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -2740,11 +2881,11 @@
       <c r="D76">
         <v>5002</v>
       </c>
-      <c r="F76" s="1" t="s">
-        <v>164</v>
+      <c r="F76" t="s">
+        <v>135</v>
       </c>
       <c r="G76">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -2760,11 +2901,11 @@
       <c r="D77">
         <v>10000</v>
       </c>
-      <c r="F77" s="1" t="s">
-        <v>165</v>
+      <c r="F77" t="s">
+        <v>133</v>
       </c>
       <c r="G77">
-        <v>47</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -2780,11 +2921,11 @@
       <c r="D78">
         <v>10000</v>
       </c>
-      <c r="F78" s="1" t="s">
-        <v>166</v>
+      <c r="F78" t="s">
+        <v>24</v>
       </c>
       <c r="G78">
-        <v>13</v>
+        <v>482</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -2800,11 +2941,11 @@
       <c r="D79">
         <v>10000</v>
       </c>
-      <c r="F79" s="1" t="s">
-        <v>167</v>
+      <c r="F79" t="s">
+        <v>136</v>
       </c>
       <c r="G79">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -2820,11 +2961,11 @@
       <c r="D80">
         <v>10000</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>168</v>
+      <c r="F80" t="s">
+        <v>277</v>
       </c>
       <c r="G80">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -2840,11 +2981,11 @@
       <c r="D81">
         <v>10000</v>
       </c>
-      <c r="F81" s="1" t="s">
-        <v>38</v>
+      <c r="F81" t="s">
+        <v>278</v>
       </c>
       <c r="G81">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -2860,11 +3001,11 @@
       <c r="D82">
         <v>6886</v>
       </c>
-      <c r="F82" s="1" t="s">
-        <v>169</v>
+      <c r="F82" t="s">
+        <v>137</v>
       </c>
       <c r="G82">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -2880,11 +3021,11 @@
       <c r="D83">
         <v>8591</v>
       </c>
-      <c r="F83" s="1" t="s">
-        <v>170</v>
+      <c r="F83" t="s">
+        <v>138</v>
       </c>
       <c r="G83">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -2900,11 +3041,11 @@
       <c r="D84">
         <v>2942</v>
       </c>
-      <c r="F84" s="1" t="s">
-        <v>171</v>
+      <c r="F84" t="s">
+        <v>139</v>
       </c>
       <c r="G84">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -2920,11 +3061,11 @@
       <c r="D85">
         <v>10000</v>
       </c>
-      <c r="F85" s="1" t="s">
-        <v>172</v>
+      <c r="F85" t="s">
+        <v>25</v>
       </c>
       <c r="G85">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -2940,11 +3081,11 @@
       <c r="D86">
         <v>9945</v>
       </c>
-      <c r="F86" s="1" t="s">
-        <v>173</v>
+      <c r="F86" t="s">
+        <v>140</v>
       </c>
       <c r="G86">
-        <v>38</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -2960,11 +3101,11 @@
       <c r="D87">
         <v>10000</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>40</v>
+      <c r="F87" t="s">
+        <v>141</v>
       </c>
       <c r="G87">
-        <v>1202</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -2980,11 +3121,11 @@
       <c r="D88">
         <v>4243</v>
       </c>
-      <c r="F88" s="1" t="s">
-        <v>174</v>
+      <c r="F88" t="s">
+        <v>142</v>
       </c>
       <c r="G88">
-        <v>34</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -3000,11 +3141,11 @@
       <c r="D89">
         <v>9781</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>175</v>
+      <c r="F89" t="s">
+        <v>279</v>
       </c>
       <c r="G89">
-        <v>3</v>
+        <v>44</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
@@ -3020,11 +3161,11 @@
       <c r="D90">
         <v>6633</v>
       </c>
-      <c r="F90" s="1" t="s">
-        <v>176</v>
+      <c r="F90" t="s">
+        <v>280</v>
       </c>
       <c r="G90">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -3040,11 +3181,11 @@
       <c r="D91">
         <v>9998</v>
       </c>
-      <c r="F91" s="1" t="s">
-        <v>177</v>
+      <c r="F91" t="s">
+        <v>143</v>
       </c>
       <c r="G91">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
@@ -3060,11 +3201,11 @@
       <c r="D92">
         <v>9998</v>
       </c>
-      <c r="F92" s="1" t="s">
-        <v>41</v>
+      <c r="F92" t="s">
+        <v>281</v>
       </c>
       <c r="G92">
-        <v>851</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -3080,11 +3221,11 @@
       <c r="D93">
         <v>9998</v>
       </c>
-      <c r="F93" s="1" t="s">
-        <v>44</v>
+      <c r="F93" t="s">
+        <v>144</v>
       </c>
       <c r="G93">
-        <v>781</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -3100,8 +3241,8 @@
       <c r="D94">
         <v>2210</v>
       </c>
-      <c r="F94" s="1" t="s">
-        <v>178</v>
+      <c r="F94" t="s">
+        <v>145</v>
       </c>
       <c r="G94">
         <v>1</v>
@@ -3120,11 +3261,11 @@
       <c r="D95">
         <v>10000</v>
       </c>
-      <c r="F95" s="1" t="s">
-        <v>179</v>
+      <c r="F95" t="s">
+        <v>26</v>
       </c>
       <c r="G95">
-        <v>1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
@@ -3140,11 +3281,11 @@
       <c r="D96">
         <v>9998</v>
       </c>
-      <c r="F96" s="1" t="s">
-        <v>46</v>
+      <c r="F96" t="s">
+        <v>146</v>
       </c>
       <c r="G96">
-        <v>336</v>
+        <v>49</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -3160,11 +3301,11 @@
       <c r="D97">
         <v>9997</v>
       </c>
-      <c r="F97" s="1" t="s">
-        <v>180</v>
+      <c r="F97" t="s">
+        <v>27</v>
       </c>
       <c r="G97">
-        <v>2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
@@ -3180,11 +3321,11 @@
       <c r="D98">
         <v>8378</v>
       </c>
-      <c r="F98" s="1" t="s">
-        <v>181</v>
+      <c r="F98" t="s">
+        <v>282</v>
       </c>
       <c r="G98">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
@@ -3200,11 +3341,11 @@
       <c r="D99">
         <v>7541</v>
       </c>
-      <c r="F99" s="1" t="s">
-        <v>182</v>
+      <c r="F99" t="s">
+        <v>28</v>
       </c>
       <c r="G99">
-        <v>20</v>
+        <v>96</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -3220,11 +3361,11 @@
       <c r="D100">
         <v>10000</v>
       </c>
-      <c r="F100" s="1" t="s">
-        <v>183</v>
+      <c r="F100" t="s">
+        <v>283</v>
       </c>
       <c r="G100">
-        <v>92</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -3240,11 +3381,11 @@
       <c r="D101">
         <v>10000</v>
       </c>
-      <c r="F101" s="1" t="s">
-        <v>184</v>
+      <c r="F101" t="s">
+        <v>147</v>
       </c>
       <c r="G101">
-        <v>258</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
@@ -3260,987 +3401,1675 @@
       <c r="D102">
         <v>10000</v>
       </c>
-      <c r="F102" s="1" t="s">
-        <v>185</v>
+      <c r="F102" t="s">
+        <v>148</v>
       </c>
       <c r="G102">
-        <v>74</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F103" s="1" t="s">
-        <v>186</v>
+      <c r="F103" t="s">
+        <v>29</v>
       </c>
       <c r="G103">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F104" s="1" t="s">
-        <v>187</v>
+      <c r="F104" t="s">
+        <v>30</v>
       </c>
       <c r="G104">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F105" t="s">
+        <v>149</v>
+      </c>
+      <c r="G105">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F106" t="s">
+        <v>31</v>
+      </c>
+      <c r="G106">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F107" t="s">
+        <v>150</v>
+      </c>
+      <c r="G107">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F108" t="s">
+        <v>32</v>
+      </c>
+      <c r="G108">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F109" t="s">
+        <v>151</v>
+      </c>
+      <c r="G109">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F110" t="s">
+        <v>284</v>
+      </c>
+      <c r="G110">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F111" t="s">
+        <v>33</v>
+      </c>
+      <c r="G111">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F112" t="s">
+        <v>152</v>
+      </c>
+      <c r="G112">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="113" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F113" t="s">
+        <v>34</v>
+      </c>
+      <c r="G113">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="114" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F114" t="s">
+        <v>153</v>
+      </c>
+      <c r="G114">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="115" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F115" t="s">
+        <v>35</v>
+      </c>
+      <c r="G115">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="116" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F116" t="s">
+        <v>285</v>
+      </c>
+      <c r="G116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F117" t="s">
+        <v>36</v>
+      </c>
+      <c r="G117">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="118" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F118" t="s">
+        <v>154</v>
+      </c>
+      <c r="G118">
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F105" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G105">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F106" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G106">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F107" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G107">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F108" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G108">
-        <v>1269</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F109" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G109">
-        <v>974</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F110" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G110">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F111" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G111">
-        <v>1054</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F112" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G112">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="113" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F113" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G113">
+    <row r="119" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F119" t="s">
+        <v>155</v>
+      </c>
+      <c r="G119">
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F114" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G114">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="115" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F115" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="G115">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="116" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F116" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G116">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="117" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F117" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="G117">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="118" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F118" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="G118">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="119" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F119" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="G119">
-        <v>7</v>
-      </c>
-    </row>
     <row r="120" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F120" s="1" t="s">
-        <v>198</v>
+      <c r="F120" t="s">
+        <v>156</v>
       </c>
       <c r="G120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F121" t="s">
+        <v>286</v>
+      </c>
+      <c r="G121">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="122" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F122" t="s">
+        <v>157</v>
+      </c>
+      <c r="G122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F123" t="s">
+        <v>287</v>
+      </c>
+      <c r="G123">
         <v>17</v>
       </c>
     </row>
-    <row r="121" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F121" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G121">
-        <v>1386</v>
-      </c>
-    </row>
-    <row r="122" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F122" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G122">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="123" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F123" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G123">
-        <v>59</v>
-      </c>
-    </row>
     <row r="124" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F124" s="1" t="s">
-        <v>200</v>
+      <c r="F124" t="s">
+        <v>158</v>
       </c>
       <c r="G124">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="125" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F125" s="1" t="s">
-        <v>201</v>
+      <c r="F125" t="s">
+        <v>288</v>
       </c>
       <c r="G125">
         <v>1</v>
       </c>
     </row>
     <row r="126" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F126" s="1" t="s">
-        <v>56</v>
+      <c r="F126" t="s">
+        <v>159</v>
       </c>
       <c r="G126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F127" t="s">
+        <v>160</v>
+      </c>
+      <c r="G127">
         <v>6</v>
       </c>
     </row>
-    <row r="127" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F127" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="G127">
-        <v>259</v>
-      </c>
-    </row>
     <row r="128" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F128" s="1" t="s">
-        <v>203</v>
+      <c r="F128" t="s">
+        <v>161</v>
       </c>
       <c r="G128">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F129" s="1" t="s">
-        <v>204</v>
+      <c r="F129" t="s">
+        <v>162</v>
       </c>
       <c r="G129">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="130" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F130" s="1" t="s">
-        <v>205</v>
+      <c r="F130" t="s">
+        <v>163</v>
       </c>
       <c r="G130">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="131" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F131" s="1" t="s">
-        <v>57</v>
+      <c r="F131" t="s">
+        <v>164</v>
       </c>
       <c r="G131">
-        <v>757</v>
+        <v>11</v>
       </c>
     </row>
     <row r="132" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F132" s="1" t="s">
-        <v>206</v>
+      <c r="F132" t="s">
+        <v>289</v>
       </c>
       <c r="G132">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F133" s="1" t="s">
-        <v>207</v>
+      <c r="F133" t="s">
+        <v>290</v>
       </c>
       <c r="G133">
         <v>3</v>
       </c>
     </row>
     <row r="134" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F134" s="1" t="s">
-        <v>58</v>
+      <c r="F134" t="s">
+        <v>37</v>
       </c>
       <c r="G134">
-        <v>133</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F135" s="1" t="s">
-        <v>208</v>
+      <c r="F135" t="s">
+        <v>38</v>
       </c>
       <c r="G135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F136" t="s">
+        <v>165</v>
+      </c>
+      <c r="G136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F137" t="s">
+        <v>166</v>
+      </c>
+      <c r="G137">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F138" t="s">
+        <v>167</v>
+      </c>
+      <c r="G138">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F139" t="s">
+        <v>168</v>
+      </c>
+      <c r="G139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F140" t="s">
+        <v>169</v>
+      </c>
+      <c r="G140">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="141" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F141" t="s">
+        <v>39</v>
+      </c>
+      <c r="G141">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="142" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F142" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G142" s="3">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="143" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F143" t="s">
+        <v>170</v>
+      </c>
+      <c r="G143">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="144" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F144" t="s">
+        <v>171</v>
+      </c>
+      <c r="G144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F145" t="s">
+        <v>291</v>
+      </c>
+      <c r="G145">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="146" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F146" t="s">
+        <v>172</v>
+      </c>
+      <c r="G146">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F147" t="s">
+        <v>173</v>
+      </c>
+      <c r="G147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F148" t="s">
+        <v>292</v>
+      </c>
+      <c r="G148">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="149" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F149" t="s">
+        <v>293</v>
+      </c>
+      <c r="G149">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="150" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F150" t="s">
+        <v>41</v>
+      </c>
+      <c r="G150">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="151" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F151" t="s">
+        <v>294</v>
+      </c>
+      <c r="G151">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="152" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F152" t="s">
+        <v>43</v>
+      </c>
+      <c r="G152">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="153" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F153" t="s">
+        <v>44</v>
+      </c>
+      <c r="G153">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="154" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F154" t="s">
+        <v>174</v>
+      </c>
+      <c r="G154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F155" t="s">
+        <v>175</v>
+      </c>
+      <c r="G155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F156" t="s">
+        <v>45</v>
+      </c>
+      <c r="G156">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="157" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F157" t="s">
+        <v>46</v>
+      </c>
+      <c r="G157">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="158" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F158" t="s">
+        <v>176</v>
+      </c>
+      <c r="G158">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F159" t="s">
+        <v>177</v>
+      </c>
+      <c r="G159">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F160" t="s">
+        <v>295</v>
+      </c>
+      <c r="G160">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="161" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F161" t="s">
+        <v>178</v>
+      </c>
+      <c r="G161">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="162" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F162" t="s">
+        <v>179</v>
+      </c>
+      <c r="G162">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="163" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F163" t="s">
+        <v>180</v>
+      </c>
+      <c r="G163">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="164" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F164" t="s">
+        <v>47</v>
+      </c>
+      <c r="G164">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="165" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F165" t="s">
+        <v>181</v>
+      </c>
+      <c r="G165">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="166" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F166" t="s">
+        <v>182</v>
+      </c>
+      <c r="G166">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="167" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F167" t="s">
+        <v>183</v>
+      </c>
+      <c r="G167">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="168" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F168" t="s">
+        <v>48</v>
+      </c>
+      <c r="G168">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="169" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F169" t="s">
+        <v>184</v>
+      </c>
+      <c r="G169">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="170" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F170" t="s">
+        <v>185</v>
+      </c>
+      <c r="G170">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="171" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F171" t="s">
+        <v>49</v>
+      </c>
+      <c r="G171">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="172" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F172" t="s">
+        <v>50</v>
+      </c>
+      <c r="G172">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="173" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F173" t="s">
+        <v>186</v>
+      </c>
+      <c r="G173">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="174" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F174" t="s">
+        <v>51</v>
+      </c>
+      <c r="G174">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="175" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F175" t="s">
+        <v>296</v>
+      </c>
+      <c r="G175">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="176" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F176" t="s">
+        <v>187</v>
+      </c>
+      <c r="G176">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="177" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F177" t="s">
+        <v>52</v>
+      </c>
+      <c r="G177">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="178" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F178" t="s">
+        <v>188</v>
+      </c>
+      <c r="G178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F179" t="s">
+        <v>297</v>
+      </c>
+      <c r="G179">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="180" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F180" t="s">
+        <v>189</v>
+      </c>
+      <c r="G180">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="181" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F181" t="s">
+        <v>190</v>
+      </c>
+      <c r="G181">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="182" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F182" t="s">
+        <v>53</v>
+      </c>
+      <c r="G182">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="183" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F183" t="s">
+        <v>191</v>
+      </c>
+      <c r="G183">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="184" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F184" t="s">
+        <v>192</v>
+      </c>
+      <c r="G184">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="185" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F185" t="s">
+        <v>298</v>
+      </c>
+      <c r="G185">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="186" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F186" t="s">
+        <v>194</v>
+      </c>
+      <c r="G186">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="187" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F187" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="136" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F136" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G136">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="137" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F137" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G137">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="138" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F138" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G138">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="139" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F139" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="G139">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="140" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F140" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G140">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="141" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F141" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="G141">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="142" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F142" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="G142">
+      <c r="G187">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="188" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F188" t="s">
+        <v>55</v>
+      </c>
+      <c r="G188">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="189" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F189" t="s">
+        <v>193</v>
+      </c>
+      <c r="G189">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="190" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F190" t="s">
+        <v>195</v>
+      </c>
+      <c r="G190">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="191" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F191" t="s">
+        <v>196</v>
+      </c>
+      <c r="G191">
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F143" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G143">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="144" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F144" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G144">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="145" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F145" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G145">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="146" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F146" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="G146">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F147" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G147">
+    <row r="192" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F192" t="s">
+        <v>56</v>
+      </c>
+      <c r="G192">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F193" t="s">
+        <v>197</v>
+      </c>
+      <c r="G193">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="194" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F194" t="s">
+        <v>198</v>
+      </c>
+      <c r="G194">
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F148" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G148">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="149" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F149" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="G149">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="150" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F150" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="G150">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="151" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F151" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G151">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="152" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F152" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G152">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="153" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F153" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G153">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="154" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F154" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="G154">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="155" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F155" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="G155">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="156" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F156" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="G156">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="157" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F157" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="G157">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="158" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F158" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G158">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="159" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F159" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="G159">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F160" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G160">
-        <v>1652</v>
-      </c>
-    </row>
-    <row r="161" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F161" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G161">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="162" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F162" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="G162">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="163" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F163" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="G163">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="164" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F164" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="G164">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="165" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F165" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G165">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="166" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F166" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="G166">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="167" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F167" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G167">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="168" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F168" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="G168">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="169" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F169" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G169">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="170" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F170" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G170">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="171" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F171" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G171">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="172" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F172" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G172">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="173" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F173" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G173">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="174" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F174" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G174">
-        <v>1749</v>
-      </c>
-    </row>
-    <row r="175" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F175" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G175">
-        <v>1315</v>
-      </c>
-    </row>
-    <row r="176" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F176" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="G176">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F177" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="G177">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="178" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F178" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G178">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="179" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F179" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="G179">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="180" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F180" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="G180">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F181" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="G181">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="182" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F182" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="G182">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="183" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F183" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G183">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="184" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F184" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G184">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="185" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F185" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="G185">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="186" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F186" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G186">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="187" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F187" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G187">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="188" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F188" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G188">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="189" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F189" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G189">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="190" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F190" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="G190">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="191" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F191" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="G191">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="192" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F192" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="G192">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="193" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F193" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G193">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="194" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F194" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="G194">
-        <v>25</v>
-      </c>
-    </row>
     <row r="195" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F195" s="1" t="s">
-        <v>86</v>
+      <c r="F195" t="s">
+        <v>199</v>
       </c>
       <c r="G195">
-        <v>366</v>
+        <v>4</v>
       </c>
     </row>
     <row r="196" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F196" s="1" t="s">
-        <v>246</v>
+      <c r="F196" t="s">
+        <v>200</v>
       </c>
       <c r="G196">
         <v>1</v>
       </c>
     </row>
     <row r="197" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F197" s="1" t="s">
+      <c r="F197" t="s">
+        <v>57</v>
+      </c>
+      <c r="G197">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="198" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F198" t="s">
+        <v>201</v>
+      </c>
+      <c r="G198">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="199" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F199" t="s">
+        <v>202</v>
+      </c>
+      <c r="G199">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F200" t="s">
+        <v>58</v>
+      </c>
+      <c r="G200">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="201" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F201" t="s">
+        <v>203</v>
+      </c>
+      <c r="G201">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="202" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F202" t="s">
+        <v>204</v>
+      </c>
+      <c r="G202">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="203" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F203" t="s">
+        <v>59</v>
+      </c>
+      <c r="G203">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F204" t="s">
+        <v>60</v>
+      </c>
+      <c r="G204">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="205" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F205" t="s">
+        <v>205</v>
+      </c>
+      <c r="G205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F206" t="s">
+        <v>61</v>
+      </c>
+      <c r="G206">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="207" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F207" t="s">
+        <v>299</v>
+      </c>
+      <c r="G207">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="208" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F208" t="s">
+        <v>62</v>
+      </c>
+      <c r="G208">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="209" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F209" t="s">
+        <v>206</v>
+      </c>
+      <c r="G209">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="210" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F210" t="s">
+        <v>207</v>
+      </c>
+      <c r="G210">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F211" t="s">
+        <v>208</v>
+      </c>
+      <c r="G211">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="212" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F212" t="s">
+        <v>63</v>
+      </c>
+      <c r="G212">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="213" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F213" t="s">
+        <v>64</v>
+      </c>
+      <c r="G213">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="214" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F214" t="s">
+        <v>300</v>
+      </c>
+      <c r="G214">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="215" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F215" t="s">
+        <v>65</v>
+      </c>
+      <c r="G215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F216" t="s">
+        <v>209</v>
+      </c>
+      <c r="G216">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="217" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F217" t="s">
+        <v>210</v>
+      </c>
+      <c r="G217">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="218" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F218" t="s">
+        <v>211</v>
+      </c>
+      <c r="G218">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="219" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F219" t="s">
+        <v>301</v>
+      </c>
+      <c r="G219">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="220" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F220" t="s">
+        <v>212</v>
+      </c>
+      <c r="G220">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="221" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F221" t="s">
+        <v>66</v>
+      </c>
+      <c r="G221">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="222" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F222" t="s">
+        <v>67</v>
+      </c>
+      <c r="G222">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="223" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F223" t="s">
+        <v>302</v>
+      </c>
+      <c r="G223">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="224" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F224" t="s">
+        <v>303</v>
+      </c>
+      <c r="G224">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="225" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F225" t="s">
+        <v>213</v>
+      </c>
+      <c r="G225">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="226" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F226" t="s">
+        <v>214</v>
+      </c>
+      <c r="G226">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="227" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F227" t="s">
+        <v>304</v>
+      </c>
+      <c r="G227">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="228" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F228" t="s">
+        <v>215</v>
+      </c>
+      <c r="G228">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="229" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F229" t="s">
+        <v>216</v>
+      </c>
+      <c r="G229">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="230" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F230" t="s">
+        <v>217</v>
+      </c>
+      <c r="G230">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="231" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F231" t="s">
+        <v>305</v>
+      </c>
+      <c r="G231">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="232" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F232" t="s">
+        <v>218</v>
+      </c>
+      <c r="G232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F233" t="s">
+        <v>306</v>
+      </c>
+      <c r="G233">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="234" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F234" t="s">
+        <v>307</v>
+      </c>
+      <c r="G234">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="235" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F235" t="s">
+        <v>308</v>
+      </c>
+      <c r="G235">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="236" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F236" t="s">
+        <v>69</v>
+      </c>
+      <c r="G236">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="237" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F237" t="s">
+        <v>70</v>
+      </c>
+      <c r="G237">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="238" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F238" t="s">
+        <v>219</v>
+      </c>
+      <c r="G238">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="239" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F239" t="s">
+        <v>220</v>
+      </c>
+      <c r="G239">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="240" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F240" t="s">
+        <v>221</v>
+      </c>
+      <c r="G240">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="241" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F241" t="s">
+        <v>222</v>
+      </c>
+      <c r="G241">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="242" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F242" t="s">
+        <v>71</v>
+      </c>
+      <c r="G242">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="243" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F243" t="s">
+        <v>223</v>
+      </c>
+      <c r="G243">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="244" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F244" t="s">
+        <v>72</v>
+      </c>
+      <c r="G244">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="245" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F245" t="s">
+        <v>224</v>
+      </c>
+      <c r="G245">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="246" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F246" t="s">
+        <v>73</v>
+      </c>
+      <c r="G246">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="247" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F247" t="s">
+        <v>309</v>
+      </c>
+      <c r="G247">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="248" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F248" t="s">
+        <v>74</v>
+      </c>
+      <c r="G248">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="249" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F249" t="s">
+        <v>75</v>
+      </c>
+      <c r="G249">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="250" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F250" t="s">
+        <v>225</v>
+      </c>
+      <c r="G250">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="251" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F251" t="s">
+        <v>310</v>
+      </c>
+      <c r="G251">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="252" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F252" t="s">
+        <v>226</v>
+      </c>
+      <c r="G252">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="253" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F253" t="s">
+        <v>76</v>
+      </c>
+      <c r="G253">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="254" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F254" t="s">
+        <v>77</v>
+      </c>
+      <c r="G254">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="255" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F255" t="s">
+        <v>311</v>
+      </c>
+      <c r="G255">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="256" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F256" t="s">
+        <v>78</v>
+      </c>
+      <c r="G256">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="257" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F257" t="s">
+        <v>227</v>
+      </c>
+      <c r="G257">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F258" t="s">
+        <v>228</v>
+      </c>
+      <c r="G258">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="259" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F259" t="s">
+        <v>229</v>
+      </c>
+      <c r="G259">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="260" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F260" t="s">
+        <v>230</v>
+      </c>
+      <c r="G260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F261" t="s">
+        <v>231</v>
+      </c>
+      <c r="G261">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="262" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F262" t="s">
+        <v>232</v>
+      </c>
+      <c r="G262">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="263" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F263" t="s">
+        <v>79</v>
+      </c>
+      <c r="G263">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="264" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F264" t="s">
+        <v>233</v>
+      </c>
+      <c r="G264">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="265" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F265" t="s">
+        <v>80</v>
+      </c>
+      <c r="G265">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="266" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F266" t="s">
+        <v>81</v>
+      </c>
+      <c r="G266">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="267" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F267" t="s">
+        <v>82</v>
+      </c>
+      <c r="G267">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="268" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F268" t="s">
+        <v>83</v>
+      </c>
+      <c r="G268">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="269" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F269" t="s">
+        <v>234</v>
+      </c>
+      <c r="G269">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="270" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F270" t="s">
+        <v>235</v>
+      </c>
+      <c r="G270">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="271" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F271" t="s">
+        <v>84</v>
+      </c>
+      <c r="G271">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="272" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F272" t="s">
+        <v>236</v>
+      </c>
+      <c r="G272">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="273" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F273" t="s">
+        <v>86</v>
+      </c>
+      <c r="G273">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="274" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F274" t="s">
+        <v>237</v>
+      </c>
+      <c r="G274">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F275" t="s">
+        <v>87</v>
+      </c>
+      <c r="G275">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="276" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F276" t="s">
+        <v>312</v>
+      </c>
+      <c r="G276">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="277" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F277" t="s">
         <v>88</v>
       </c>
-      <c r="G197">
-        <v>1552</v>
-      </c>
-    </row>
-    <row r="198" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F198" s="1" t="s">
+      <c r="G277">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="278" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F278" t="s">
+        <v>89</v>
+      </c>
+      <c r="G278">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="279" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F279" t="s">
+        <v>238</v>
+      </c>
+      <c r="G279">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="280" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F280" t="s">
+        <v>239</v>
+      </c>
+      <c r="G280">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="281" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F281" t="s">
+        <v>240</v>
+      </c>
+      <c r="G281">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="282" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F282" t="s">
+        <v>241</v>
+      </c>
+      <c r="G282">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="283" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F283" t="s">
+        <v>90</v>
+      </c>
+      <c r="G283">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="284" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F284" t="s">
+        <v>313</v>
+      </c>
+      <c r="G284">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="285" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F285" t="s">
+        <v>242</v>
+      </c>
+      <c r="G285">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F286" t="s">
+        <v>243</v>
+      </c>
+      <c r="G286">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="287" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F287" t="s">
+        <v>244</v>
+      </c>
+      <c r="G287">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F288" t="s">
+        <v>314</v>
+      </c>
+      <c r="G288">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="289" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F289" t="s">
+        <v>91</v>
+      </c>
+      <c r="G289">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="290" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F290" t="s">
+        <v>92</v>
+      </c>
+      <c r="G290">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="291" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F291" t="s">
+        <v>245</v>
+      </c>
+      <c r="G291">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="292" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F292" t="s">
+        <v>246</v>
+      </c>
+      <c r="G292">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="293" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F293" t="s">
         <v>247</v>
       </c>
-      <c r="G198">
+      <c r="G293">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F294" t="s">
+        <v>93</v>
+      </c>
+      <c r="G294">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="295" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F295" t="s">
+        <v>248</v>
+      </c>
+      <c r="G295">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="296" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F296" t="s">
+        <v>315</v>
+      </c>
+      <c r="G296">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="297" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F297" t="s">
+        <v>94</v>
+      </c>
+      <c r="G297">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="298" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F298" t="s">
+        <v>95</v>
+      </c>
+      <c r="G298">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="299" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F299" t="s">
+        <v>249</v>
+      </c>
+      <c r="G299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F300" t="s">
+        <v>250</v>
+      </c>
+      <c r="G300">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="301" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F301" t="s">
+        <v>251</v>
+      </c>
+      <c r="G301">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="302" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F302" t="s">
+        <v>252</v>
+      </c>
+      <c r="G302">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F303" t="s">
+        <v>316</v>
+      </c>
+      <c r="G303">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="304" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F304" t="s">
+        <v>253</v>
+      </c>
+      <c r="G304">
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F199" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="G199">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="200" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F200" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="G200">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="201" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F201" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="G201">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="202" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F202" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G202">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="203" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F203" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="G203">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="204" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F204" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="G204">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="205" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F205" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="G205">
+    <row r="305" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F305" t="s">
+        <v>317</v>
+      </c>
+      <c r="G305">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="306" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F306" t="s">
+        <v>97</v>
+      </c>
+      <c r="G306">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="307" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F307" t="s">
+        <v>254</v>
+      </c>
+      <c r="G307">
         <v>11</v>
       </c>
     </row>
-    <row r="206" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F206" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G206">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="207" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F207" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G207">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="208" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F208" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="G208">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="209" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F209" s="1" t="s">
+    <row r="308" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F308" t="s">
         <v>255</v>
       </c>
-      <c r="G209">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="210" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F210" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="G210">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="211" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F211" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="G211">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="212" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F212" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G212">
-        <v>1396</v>
-      </c>
-    </row>
-    <row r="213" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F213" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G213">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="214" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F214" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="G214">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="215" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F215" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G215">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="216" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F216" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="G216">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="217" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F217" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="G217">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="218" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F218" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="G218">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="219" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F219" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="G219">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="220" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F220" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G220">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="221" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F221" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="G221">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="222" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F222" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G222">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="223" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F223" s="1" t="s">
+      <c r="G308">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="309" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F309" t="s">
         <v>98</v>
       </c>
-      <c r="G223">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="224" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F224" s="1" t="s">
+      <c r="G309">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="310" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F310" t="s">
         <v>99</v>
       </c>
-      <c r="G224">
-        <v>46</v>
+      <c r="G310">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>